<commit_message>
giving jack access to minmax. CB = Caribbean, CA = Central America, SA = South America. All flights from JFK
</commit_message>
<xml_diff>
--- a/data/YHack prices_1.xlsx
+++ b/data/YHack prices_1.xlsx
@@ -48,7 +48,7 @@
     <t xml:space="preserve">CUR</t>
   </si>
   <si>
-    <t xml:space="preserve">CGM</t>
+    <t xml:space="preserve">GCM</t>
   </si>
   <si>
     <t xml:space="preserve">GND</t>
@@ -631,7 +631,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A2:AZ23"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -657,7 +657,7 @@
   <dimension ref="A1:AZ51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:AZ23"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5560,7 +5560,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="A2:AZ23"/>
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>